<commit_message>
Updating Frag. 1 a
</commit_message>
<xml_diff>
--- a/Digital_Editions/4Q266/457_1239_Frg_1_a/457_1239.xlsx
+++ b/Digital_Editions/4Q266/457_1239_Frg_1_a/457_1239.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/bkp/editions/Damascus_edition/4Q266/Frg_1_a/Frg_1_a_א/iaa_images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tucker-James/github/SQE-Damascus/Digital_Editions/4Q266/457_1239_Frg_1_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B6FF9-9B17-9E49-82B3-927175BE39FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99350B2F-C5DE-5C46-8B74-70B039B50EBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="21860" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="258">
   <si>
     <t>id</t>
   </si>
@@ -794,6 +794,15 @@
   </si>
   <si>
     <t>פ</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>112-113-114-115</t>
+  </si>
+  <si>
+    <t>The scribe likely started to erase the word after realizing he created a parablepsis (skipping a line). He then likely decided to erase the word altogether</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1189,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q164" sqref="Q164"/>
+      <selection pane="bottomLeft" activeCell="V157" sqref="V157:X161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5938,6 +5947,24 @@
         <f>SIGNs!A106</f>
         <v>105</v>
       </c>
+      <c r="G112">
+        <v>99</v>
+      </c>
+      <c r="K112" t="b">
+        <v>0</v>
+      </c>
+      <c r="L112" t="b">
+        <v>0</v>
+      </c>
+      <c r="M112" t="b">
+        <v>0</v>
+      </c>
+      <c r="N112" t="b">
+        <v>0</v>
+      </c>
+      <c r="O112" t="s">
+        <v>209</v>
+      </c>
       <c r="P112">
         <v>0</v>
       </c>
@@ -5947,165 +5974,582 @@
       <c r="U112">
         <v>15</v>
       </c>
-    </row>
-    <row r="113" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="V112" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W112" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X112" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C113">
         <f>SIGNs!A107</f>
         <v>106</v>
       </c>
+      <c r="G113">
+        <v>100</v>
+      </c>
+      <c r="K113" t="b">
+        <v>0</v>
+      </c>
+      <c r="L113" t="b">
+        <v>0</v>
+      </c>
+      <c r="M113" t="b">
+        <v>0</v>
+      </c>
+      <c r="N113" t="b">
+        <v>0</v>
+      </c>
+      <c r="O113" t="s">
+        <v>209</v>
+      </c>
       <c r="P113">
         <v>0</v>
       </c>
       <c r="Q113" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="114" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U113">
+        <v>15</v>
+      </c>
+      <c r="V113" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W113" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X113" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="114" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C114">
         <f>SIGNs!A108</f>
         <v>107</v>
       </c>
+      <c r="G114">
+        <v>101</v>
+      </c>
+      <c r="K114" t="b">
+        <v>0</v>
+      </c>
+      <c r="L114" t="b">
+        <v>0</v>
+      </c>
+      <c r="M114" t="b">
+        <v>0</v>
+      </c>
+      <c r="N114" t="b">
+        <v>0</v>
+      </c>
+      <c r="O114" t="s">
+        <v>209</v>
+      </c>
       <c r="P114">
         <v>0</v>
       </c>
       <c r="Q114" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="115" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U114">
+        <v>15</v>
+      </c>
+      <c r="V114" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W114" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X114" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C115">
         <f>SIGNs!A109</f>
         <v>108</v>
       </c>
+      <c r="G115">
+        <v>102</v>
+      </c>
+      <c r="K115" t="b">
+        <v>0</v>
+      </c>
+      <c r="L115" t="b">
+        <v>1</v>
+      </c>
+      <c r="M115" t="b">
+        <v>0</v>
+      </c>
+      <c r="N115" t="b">
+        <v>0</v>
+      </c>
+      <c r="O115" t="s">
+        <v>209</v>
+      </c>
       <c r="P115">
         <v>0</v>
       </c>
       <c r="Q115" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="116" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U115">
+        <v>15</v>
+      </c>
+      <c r="V115" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W115" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X115" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="116" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C116">
         <f>SIGNs!A110</f>
         <v>109</v>
       </c>
+      <c r="G116">
+        <v>103</v>
+      </c>
+      <c r="K116" t="b">
+        <v>0</v>
+      </c>
+      <c r="L116" t="b">
+        <v>0</v>
+      </c>
+      <c r="M116" t="b">
+        <v>0</v>
+      </c>
+      <c r="N116" t="b">
+        <v>0</v>
+      </c>
+      <c r="O116" t="s">
+        <v>209</v>
+      </c>
       <c r="P116">
         <v>0</v>
       </c>
       <c r="Q116" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="117" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U116">
+        <v>15</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W116" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X116" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C117">
         <f>SIGNs!A111</f>
         <v>110</v>
       </c>
+      <c r="G117">
+        <v>104</v>
+      </c>
+      <c r="K117" t="b">
+        <v>0</v>
+      </c>
+      <c r="L117" t="s">
+        <v>218</v>
+      </c>
+      <c r="M117" t="b">
+        <v>0</v>
+      </c>
+      <c r="N117" t="b">
+        <v>0</v>
+      </c>
+      <c r="O117" t="s">
+        <v>218</v>
+      </c>
       <c r="P117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U117">
+        <v>15</v>
+      </c>
+      <c r="V117" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W117" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X117" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="118" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C118">
         <f>SIGNs!A112</f>
         <v>111</v>
       </c>
+      <c r="G118">
+        <v>105</v>
+      </c>
+      <c r="K118" t="b">
+        <v>0</v>
+      </c>
+      <c r="L118" t="b">
+        <v>1</v>
+      </c>
+      <c r="M118" t="b">
+        <v>0</v>
+      </c>
+      <c r="N118" t="b">
+        <v>0</v>
+      </c>
+      <c r="O118" t="s">
+        <v>209</v>
+      </c>
       <c r="P118">
         <v>0</v>
       </c>
       <c r="Q118" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="119" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U118">
+        <v>15</v>
+      </c>
+      <c r="V118" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W118" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X118" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C119">
         <f>SIGNs!A113</f>
         <v>112</v>
       </c>
+      <c r="G119">
+        <v>106</v>
+      </c>
+      <c r="K119" t="b">
+        <v>0</v>
+      </c>
+      <c r="L119" t="b">
+        <v>1</v>
+      </c>
+      <c r="M119" t="b">
+        <v>0</v>
+      </c>
+      <c r="N119" t="b">
+        <v>0</v>
+      </c>
+      <c r="O119" t="s">
+        <v>209</v>
+      </c>
       <c r="P119">
         <v>0</v>
       </c>
       <c r="Q119" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="120" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U119">
+        <v>15</v>
+      </c>
+      <c r="V119" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W119" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X119" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C120">
         <f>SIGNs!A114</f>
         <v>113</v>
       </c>
+      <c r="G120">
+        <v>107</v>
+      </c>
+      <c r="K120" t="b">
+        <v>0</v>
+      </c>
+      <c r="L120" t="b">
+        <v>1</v>
+      </c>
+      <c r="M120" t="b">
+        <v>0</v>
+      </c>
+      <c r="N120" t="b">
+        <v>0</v>
+      </c>
+      <c r="O120" t="s">
+        <v>209</v>
+      </c>
       <c r="P120">
         <v>0</v>
       </c>
       <c r="Q120" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="121" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U120">
+        <v>15</v>
+      </c>
+      <c r="V120" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W120" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X120" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="121" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C121">
         <f>SIGNs!A115</f>
         <v>114</v>
       </c>
+      <c r="G121">
+        <v>108</v>
+      </c>
+      <c r="K121" t="b">
+        <v>0</v>
+      </c>
+      <c r="L121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M121" t="b">
+        <v>0</v>
+      </c>
+      <c r="N121" t="b">
+        <v>1</v>
+      </c>
+      <c r="O121" t="s">
+        <v>209</v>
+      </c>
       <c r="P121">
         <v>0</v>
       </c>
       <c r="Q121" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="122" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U121">
+        <v>15</v>
+      </c>
+      <c r="V121" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W121" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X121" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="122" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C122">
         <f>SIGNs!A116</f>
         <v>115</v>
       </c>
+      <c r="G122">
+        <v>109</v>
+      </c>
+      <c r="K122" t="b">
+        <v>0</v>
+      </c>
+      <c r="L122" t="b">
+        <v>1</v>
+      </c>
+      <c r="M122" t="b">
+        <v>0</v>
+      </c>
+      <c r="N122" t="b">
+        <v>0</v>
+      </c>
+      <c r="O122" t="s">
+        <v>209</v>
+      </c>
       <c r="P122">
         <v>0</v>
       </c>
       <c r="Q122" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="123" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U122">
+        <v>15</v>
+      </c>
+      <c r="V122" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W122" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X122" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="123" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C123">
         <f>SIGNs!A117</f>
         <v>116</v>
       </c>
+      <c r="G123">
+        <v>110</v>
+      </c>
+      <c r="K123" t="b">
+        <v>0</v>
+      </c>
+      <c r="L123" t="b">
+        <v>1</v>
+      </c>
+      <c r="M123" t="b">
+        <v>1</v>
+      </c>
+      <c r="N123" t="b">
+        <v>1</v>
+      </c>
+      <c r="O123" t="s">
+        <v>205</v>
+      </c>
       <c r="P123">
         <v>0</v>
       </c>
       <c r="Q123" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="124" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U123">
+        <v>15</v>
+      </c>
+      <c r="V123" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W123" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X123" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="124" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C124">
         <f>SIGNs!A118</f>
         <v>117</v>
       </c>
+      <c r="G124">
+        <v>111</v>
+      </c>
+      <c r="K124" t="b">
+        <v>1</v>
+      </c>
+      <c r="L124" t="b">
+        <v>0</v>
+      </c>
+      <c r="M124" t="b">
+        <v>1</v>
+      </c>
+      <c r="N124" t="b">
+        <v>1</v>
+      </c>
+      <c r="O124" t="s">
+        <v>205</v>
+      </c>
       <c r="P124">
         <v>0</v>
       </c>
       <c r="Q124" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="125" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U124">
+        <v>15</v>
+      </c>
+      <c r="V124" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W124" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X124" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="125" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C125">
         <f>SIGNs!A119</f>
         <v>118</v>
       </c>
+      <c r="G125">
+        <v>111</v>
+      </c>
+      <c r="K125" t="b">
+        <v>1</v>
+      </c>
+      <c r="L125" t="b">
+        <v>0</v>
+      </c>
+      <c r="M125" t="b">
+        <v>1</v>
+      </c>
+      <c r="N125" t="b">
+        <v>1</v>
+      </c>
+      <c r="O125" t="s">
+        <v>205</v>
+      </c>
       <c r="P125">
         <v>0</v>
       </c>
       <c r="Q125" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="126" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U125">
+        <v>15</v>
+      </c>
+      <c r="V125" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W125" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X125" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="126" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C126">
         <f>SIGNs!A120</f>
         <v>119</v>
       </c>
+      <c r="G126">
+        <v>112</v>
+      </c>
+      <c r="K126" t="b">
+        <v>0</v>
+      </c>
+      <c r="L126" t="s">
+        <v>218</v>
+      </c>
+      <c r="M126" t="b">
+        <v>1</v>
+      </c>
+      <c r="N126" t="b">
+        <v>1</v>
+      </c>
+      <c r="O126" t="s">
+        <v>207</v>
+      </c>
       <c r="P126">
         <v>0</v>
       </c>
@@ -6115,174 +6559,627 @@
       <c r="U126">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="V126" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W126" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X126" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="127" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C127">
         <f>SIGNs!A121</f>
         <v>120</v>
       </c>
+      <c r="G127">
+        <v>113</v>
+      </c>
+      <c r="K127" t="b">
+        <v>0</v>
+      </c>
+      <c r="L127" t="s">
+        <v>218</v>
+      </c>
+      <c r="M127" t="b">
+        <v>1</v>
+      </c>
+      <c r="N127" t="b">
+        <v>1</v>
+      </c>
+      <c r="O127" t="s">
+        <v>207</v>
+      </c>
       <c r="P127">
         <v>0</v>
       </c>
       <c r="Q127" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="128" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U127">
+        <v>16</v>
+      </c>
+      <c r="V127" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X127" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="128" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C128">
         <f>SIGNs!A122</f>
         <v>121</v>
       </c>
+      <c r="G128">
+        <v>114</v>
+      </c>
+      <c r="K128" t="b">
+        <v>0</v>
+      </c>
+      <c r="L128" t="s">
+        <v>218</v>
+      </c>
+      <c r="M128" t="b">
+        <v>1</v>
+      </c>
+      <c r="N128" t="b">
+        <v>1</v>
+      </c>
+      <c r="O128" t="s">
+        <v>207</v>
+      </c>
       <c r="P128">
         <v>0</v>
       </c>
       <c r="Q128" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="129" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U128">
+        <v>16</v>
+      </c>
+      <c r="V128" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W128" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X128" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="129" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C129">
         <f>SIGNs!A123</f>
         <v>122</v>
       </c>
+      <c r="G129">
+        <v>115</v>
+      </c>
+      <c r="K129" t="s">
+        <v>218</v>
+      </c>
+      <c r="L129" t="s">
+        <v>218</v>
+      </c>
+      <c r="M129" t="s">
+        <v>218</v>
+      </c>
+      <c r="N129" t="s">
+        <v>218</v>
+      </c>
+      <c r="O129" t="s">
+        <v>218</v>
+      </c>
       <c r="P129">
         <v>0</v>
       </c>
       <c r="Q129" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="130" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U129">
+        <v>16</v>
+      </c>
+      <c r="V129" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W129" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X129" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C130">
         <f>SIGNs!A124</f>
         <v>123</v>
       </c>
+      <c r="G130">
+        <v>116</v>
+      </c>
+      <c r="J130" t="s">
+        <v>256</v>
+      </c>
+      <c r="K130" t="s">
+        <v>218</v>
+      </c>
+      <c r="L130" t="s">
+        <v>218</v>
+      </c>
+      <c r="M130" t="s">
+        <v>218</v>
+      </c>
+      <c r="N130" t="s">
+        <v>218</v>
+      </c>
+      <c r="O130" t="s">
+        <v>218</v>
+      </c>
       <c r="P130">
         <v>0</v>
       </c>
       <c r="Q130" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="131" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U130">
+        <v>16</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W130" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X130" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="131" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C131">
+        <f>SIGNs!A160</f>
+        <v>159</v>
+      </c>
+      <c r="G131">
+        <v>117</v>
+      </c>
+      <c r="K131" t="b">
+        <v>0</v>
+      </c>
+      <c r="L131" t="s">
+        <v>218</v>
+      </c>
+      <c r="M131" t="b">
+        <v>0</v>
+      </c>
+      <c r="N131" t="b">
+        <v>0</v>
+      </c>
+      <c r="O131" t="s">
+        <v>218</v>
+      </c>
+      <c r="P131">
+        <v>0</v>
+      </c>
+      <c r="U131">
+        <v>16</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X131" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="132" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C132">
         <f>SIGNs!A125</f>
         <v>124</v>
       </c>
-      <c r="P131">
-        <v>0</v>
-      </c>
-      <c r="Q131" t="s">
+      <c r="G132">
+        <v>118</v>
+      </c>
+      <c r="K132" t="b">
+        <v>0</v>
+      </c>
+      <c r="L132" t="b">
+        <v>0</v>
+      </c>
+      <c r="M132" t="b">
+        <v>0</v>
+      </c>
+      <c r="N132" t="b">
+        <v>1</v>
+      </c>
+      <c r="O132" t="s">
+        <v>205</v>
+      </c>
+      <c r="P132">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="132" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C132">
+      <c r="U132">
+        <v>16</v>
+      </c>
+      <c r="V132" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W132" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X132" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="133" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C133">
         <f>SIGNs!A126</f>
         <v>125</v>
       </c>
-      <c r="P132">
-        <v>0</v>
-      </c>
-      <c r="Q132" t="s">
+      <c r="G133">
+        <v>119</v>
+      </c>
+      <c r="K133" t="b">
+        <v>0</v>
+      </c>
+      <c r="L133" t="b">
+        <v>0</v>
+      </c>
+      <c r="M133" t="b">
+        <v>0</v>
+      </c>
+      <c r="N133" t="b">
+        <v>1</v>
+      </c>
+      <c r="O133" t="s">
+        <v>209</v>
+      </c>
+      <c r="P133">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="133" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C133">
+      <c r="U133">
+        <v>16</v>
+      </c>
+      <c r="V133" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W133" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X133" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="134" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C134">
         <f>SIGNs!A127</f>
         <v>126</v>
       </c>
-      <c r="P133">
-        <v>0</v>
-      </c>
-      <c r="Q133" t="s">
+      <c r="G134">
+        <v>120</v>
+      </c>
+      <c r="K134" t="b">
+        <v>0</v>
+      </c>
+      <c r="L134" t="b">
+        <v>0</v>
+      </c>
+      <c r="M134" t="b">
+        <v>0</v>
+      </c>
+      <c r="N134" t="b">
+        <v>0</v>
+      </c>
+      <c r="O134" t="s">
+        <v>205</v>
+      </c>
+      <c r="P134">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="s">
         <v>231</v>
       </c>
-      <c r="R133" t="s">
+      <c r="R134" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="134" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C134">
+      <c r="U134">
+        <v>16</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="135" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C135">
         <f>SIGNs!A128</f>
         <v>127</v>
       </c>
-      <c r="P134">
-        <v>0</v>
-      </c>
-      <c r="Q134" t="s">
+      <c r="G135">
+        <v>121</v>
+      </c>
+      <c r="K135" t="b">
+        <v>0</v>
+      </c>
+      <c r="L135" t="b">
+        <v>0</v>
+      </c>
+      <c r="M135" t="b">
+        <v>0</v>
+      </c>
+      <c r="N135" t="b">
+        <v>1</v>
+      </c>
+      <c r="O135" t="s">
+        <v>209</v>
+      </c>
+      <c r="P135">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="135" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C135">
+      <c r="U135">
+        <v>16</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X135" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="136" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C136">
         <f>SIGNs!A129</f>
         <v>128</v>
       </c>
-      <c r="P135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C136">
-        <f>SIGNs!A130</f>
-        <v>129</v>
+      <c r="G136">
+        <v>122</v>
+      </c>
+      <c r="K136" t="s">
+        <v>218</v>
+      </c>
+      <c r="L136" t="s">
+        <v>218</v>
+      </c>
+      <c r="M136" t="b">
+        <v>0</v>
+      </c>
+      <c r="N136" t="b">
+        <v>1</v>
+      </c>
+      <c r="O136" t="s">
+        <v>218</v>
       </c>
       <c r="P136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U136">
+        <v>16</v>
+      </c>
+      <c r="V136" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W136" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X136" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="137" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C137">
-        <f>SIGNs!A131</f>
-        <v>130</v>
-      </c>
-      <c r="P137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C138">
         <f>SIGNs!A132</f>
         <v>131</v>
       </c>
-      <c r="P138">
-        <v>0</v>
-      </c>
-      <c r="Q138" t="s">
+      <c r="G137">
+        <v>123</v>
+      </c>
+      <c r="K137" t="b">
+        <v>0</v>
+      </c>
+      <c r="L137" t="b">
+        <v>0</v>
+      </c>
+      <c r="M137" t="b">
+        <v>0</v>
+      </c>
+      <c r="N137" t="b">
+        <v>1</v>
+      </c>
+      <c r="O137" t="s">
+        <v>209</v>
+      </c>
+      <c r="P137">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="139" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C139">
+      <c r="U137">
+        <v>16</v>
+      </c>
+      <c r="V137" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W137" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X137" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="138" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C138">
         <f>SIGNs!A133</f>
         <v>132</v>
       </c>
+      <c r="G138">
+        <v>124</v>
+      </c>
+      <c r="K138" t="b">
+        <v>0</v>
+      </c>
+      <c r="L138" t="b">
+        <v>0</v>
+      </c>
+      <c r="M138" t="b">
+        <v>0</v>
+      </c>
+      <c r="N138" t="b">
+        <v>0</v>
+      </c>
+      <c r="O138" t="s">
+        <v>209</v>
+      </c>
+      <c r="P138">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>208</v>
+      </c>
+      <c r="U138">
+        <v>16</v>
+      </c>
+      <c r="V138" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W138" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X138" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="139" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <f>SIGNs!A164</f>
+        <v>163</v>
+      </c>
+      <c r="G139">
+        <v>125</v>
+      </c>
+      <c r="K139" t="s">
+        <v>218</v>
+      </c>
+      <c r="L139" t="s">
+        <v>218</v>
+      </c>
+      <c r="M139" t="b">
+        <v>0</v>
+      </c>
+      <c r="N139" t="b">
+        <v>0</v>
+      </c>
+      <c r="O139" t="s">
+        <v>218</v>
+      </c>
       <c r="P139">
         <v>0</v>
       </c>
-      <c r="Q139" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="140" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U139">
+        <v>16</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W139" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X139" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="140" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C140">
         <f>SIGNs!A134</f>
         <v>133</v>
       </c>
+      <c r="G140">
+        <v>126</v>
+      </c>
+      <c r="K140" t="b">
+        <v>0</v>
+      </c>
+      <c r="L140" t="s">
+        <v>218</v>
+      </c>
+      <c r="M140" t="b">
+        <v>1</v>
+      </c>
+      <c r="N140" t="b">
+        <v>1</v>
+      </c>
+      <c r="O140" t="s">
+        <v>207</v>
+      </c>
       <c r="P140">
         <v>0</v>
       </c>
       <c r="Q140" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="141" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U140">
+        <v>16</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W140" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X140" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="141" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C141">
         <f>SIGNs!A135</f>
         <v>134</v>
       </c>
+      <c r="G141">
+        <v>127</v>
+      </c>
+      <c r="K141" t="b">
+        <v>0</v>
+      </c>
+      <c r="L141" t="b">
+        <v>0</v>
+      </c>
+      <c r="M141" t="b">
+        <v>0</v>
+      </c>
+      <c r="N141" t="b">
+        <v>0</v>
+      </c>
+      <c r="O141" t="s">
+        <v>209</v>
+      </c>
       <c r="P141">
         <v>0</v>
       </c>
@@ -6292,140 +7189,497 @@
       <c r="U141">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="V141" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W141" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X141" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="142" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C142">
         <f>SIGNs!A136</f>
         <v>135</v>
       </c>
+      <c r="G142">
+        <v>128</v>
+      </c>
+      <c r="K142" t="b">
+        <v>0</v>
+      </c>
+      <c r="L142" t="b">
+        <v>0</v>
+      </c>
+      <c r="M142" t="b">
+        <v>0</v>
+      </c>
+      <c r="N142" t="b">
+        <v>0</v>
+      </c>
+      <c r="O142" t="s">
+        <v>209</v>
+      </c>
       <c r="P142">
         <v>0</v>
       </c>
       <c r="Q142" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="143" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U142">
+        <v>17</v>
+      </c>
+      <c r="V142" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W142" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X142" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="143" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C143">
         <f>SIGNs!A137</f>
         <v>136</v>
       </c>
+      <c r="G143">
+        <v>129</v>
+      </c>
+      <c r="K143" t="b">
+        <v>0</v>
+      </c>
+      <c r="L143" t="b">
+        <v>1</v>
+      </c>
+      <c r="M143" t="b">
+        <v>0</v>
+      </c>
+      <c r="N143" t="b">
+        <v>0</v>
+      </c>
+      <c r="O143" t="s">
+        <v>209</v>
+      </c>
       <c r="P143">
         <v>0</v>
       </c>
       <c r="Q143" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="144" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U143">
+        <v>17</v>
+      </c>
+      <c r="V143" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W143" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X143" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="144" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C144">
         <f>SIGNs!A138</f>
         <v>137</v>
       </c>
+      <c r="G144">
+        <v>130</v>
+      </c>
+      <c r="K144" t="b">
+        <v>0</v>
+      </c>
+      <c r="L144" t="b">
+        <v>0</v>
+      </c>
+      <c r="M144" t="b">
+        <v>0</v>
+      </c>
+      <c r="N144" t="b">
+        <v>0</v>
+      </c>
+      <c r="O144" t="s">
+        <v>209</v>
+      </c>
       <c r="P144">
         <v>0</v>
       </c>
       <c r="Q144" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="145" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U144">
+        <v>17</v>
+      </c>
+      <c r="V144" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W144" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X144" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="145" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C145">
         <f>SIGNs!A139</f>
         <v>138</v>
       </c>
+      <c r="G145">
+        <v>131</v>
+      </c>
+      <c r="K145" t="s">
+        <v>218</v>
+      </c>
+      <c r="L145" t="s">
+        <v>218</v>
+      </c>
+      <c r="M145" t="b">
+        <v>0</v>
+      </c>
+      <c r="N145" t="b">
+        <v>0</v>
+      </c>
+      <c r="O145" t="s">
+        <v>218</v>
+      </c>
       <c r="P145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U145">
+        <v>17</v>
+      </c>
+      <c r="V145" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W145" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X145" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="146" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C146">
         <f>SIGNs!A140</f>
         <v>139</v>
       </c>
+      <c r="G146">
+        <v>132</v>
+      </c>
+      <c r="K146" t="b">
+        <v>0</v>
+      </c>
+      <c r="L146" t="s">
+        <v>218</v>
+      </c>
+      <c r="M146" t="b">
+        <v>1</v>
+      </c>
+      <c r="N146" t="b">
+        <v>1</v>
+      </c>
+      <c r="O146" t="s">
+        <v>218</v>
+      </c>
       <c r="P146">
         <v>0</v>
       </c>
       <c r="Q146" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="147" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U146">
+        <v>17</v>
+      </c>
+      <c r="V146" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W146" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X146" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="147" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C147">
         <f>SIGNs!A141</f>
         <v>140</v>
       </c>
+      <c r="G147">
+        <v>133</v>
+      </c>
+      <c r="K147" t="b">
+        <v>0</v>
+      </c>
+      <c r="L147" t="b">
+        <v>1</v>
+      </c>
+      <c r="M147" t="b">
+        <v>1</v>
+      </c>
+      <c r="N147" t="b">
+        <v>1</v>
+      </c>
+      <c r="O147" t="s">
+        <v>207</v>
+      </c>
       <c r="P147">
         <v>0</v>
       </c>
       <c r="Q147" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="148" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U147">
+        <v>17</v>
+      </c>
+      <c r="V147" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W147" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X147" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="148" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C148">
         <f>SIGNs!A142</f>
         <v>141</v>
       </c>
+      <c r="G148">
+        <v>134</v>
+      </c>
+      <c r="K148" t="b">
+        <v>0</v>
+      </c>
+      <c r="L148" t="b">
+        <v>0</v>
+      </c>
+      <c r="M148" t="b">
+        <v>0</v>
+      </c>
+      <c r="N148" t="b">
+        <v>0</v>
+      </c>
+      <c r="O148" t="s">
+        <v>205</v>
+      </c>
       <c r="P148">
         <v>0</v>
       </c>
       <c r="Q148" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="149" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U148">
+        <v>17</v>
+      </c>
+      <c r="V148" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W148" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X148" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="149" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C149">
         <f>SIGNs!A143</f>
         <v>142</v>
       </c>
+      <c r="G149">
+        <v>135</v>
+      </c>
+      <c r="K149" t="b">
+        <v>0</v>
+      </c>
+      <c r="L149" t="b">
+        <v>0</v>
+      </c>
+      <c r="M149" t="b">
+        <v>1</v>
+      </c>
+      <c r="N149" t="b">
+        <v>1</v>
+      </c>
+      <c r="O149" t="s">
+        <v>218</v>
+      </c>
       <c r="P149">
         <v>0</v>
       </c>
       <c r="Q149" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="150" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U149">
+        <v>17</v>
+      </c>
+      <c r="V149" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W149" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X149" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="150" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C150">
         <f>SIGNs!A144</f>
         <v>143</v>
       </c>
+      <c r="G150">
+        <v>136</v>
+      </c>
+      <c r="K150" t="s">
+        <v>218</v>
+      </c>
+      <c r="L150" t="s">
+        <v>218</v>
+      </c>
+      <c r="M150" t="b">
+        <v>1</v>
+      </c>
+      <c r="N150" t="b">
+        <v>1</v>
+      </c>
+      <c r="O150" t="s">
+        <v>218</v>
+      </c>
       <c r="P150">
         <v>0</v>
       </c>
       <c r="Q150" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="151" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U150">
+        <v>17</v>
+      </c>
+      <c r="V150" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W150" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X150" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="151" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C151">
         <f>SIGNs!A145</f>
         <v>144</v>
       </c>
+      <c r="G151">
+        <v>137</v>
+      </c>
+      <c r="K151" t="b">
+        <v>0</v>
+      </c>
+      <c r="L151" t="b">
+        <v>0</v>
+      </c>
+      <c r="M151" t="s">
+        <v>212</v>
+      </c>
+      <c r="N151" t="b">
+        <v>1</v>
+      </c>
+      <c r="O151" t="s">
+        <v>209</v>
+      </c>
       <c r="P151">
         <v>0</v>
       </c>
       <c r="Q151" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="152" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U151">
+        <v>17</v>
+      </c>
+      <c r="V151" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W151" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X151" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="152" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C152">
+        <f>SIGNs!A147</f>
+        <v>146</v>
+      </c>
+      <c r="G152">
+        <v>138</v>
+      </c>
+      <c r="K152" t="s">
+        <v>218</v>
+      </c>
+      <c r="L152" t="s">
+        <v>218</v>
+      </c>
+      <c r="M152" t="b">
+        <v>1</v>
+      </c>
+      <c r="N152" t="b">
+        <v>1</v>
+      </c>
+      <c r="O152" t="s">
+        <v>218</v>
+      </c>
+      <c r="P152">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>229</v>
+      </c>
+      <c r="U152">
+        <v>17</v>
+      </c>
+      <c r="V152" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W152" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X152" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="153" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C153">
         <f>SIGNs!A146</f>
         <v>145</v>
       </c>
-      <c r="P152">
-        <v>0</v>
-      </c>
-      <c r="Q152" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="153" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C153">
-        <f>SIGNs!A147</f>
-        <v>146</v>
+      <c r="G153">
+        <v>139</v>
+      </c>
+      <c r="K153" t="s">
+        <v>218</v>
+      </c>
+      <c r="L153" t="s">
+        <v>218</v>
+      </c>
+      <c r="M153" t="b">
+        <v>1</v>
+      </c>
+      <c r="N153" t="b">
+        <v>1</v>
+      </c>
+      <c r="O153" t="s">
+        <v>218</v>
       </c>
       <c r="P153">
         <v>0</v>
@@ -6433,173 +7687,395 @@
       <c r="Q153" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="154" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U153">
+        <v>17</v>
+      </c>
+      <c r="V153" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W153" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X153" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="154" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C154">
         <f>SIGNs!A148</f>
         <v>147</v>
       </c>
+      <c r="G154">
+        <v>140</v>
+      </c>
+      <c r="K154" t="s">
+        <v>218</v>
+      </c>
+      <c r="L154" t="b">
+        <v>0</v>
+      </c>
+      <c r="M154" t="b">
+        <v>1</v>
+      </c>
+      <c r="N154" t="b">
+        <v>1</v>
+      </c>
+      <c r="O154" t="s">
+        <v>218</v>
+      </c>
       <c r="P154">
         <v>0</v>
       </c>
       <c r="Q154" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="155" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="U154">
+        <v>17</v>
+      </c>
+      <c r="V154" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W154" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X154" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="155" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C155">
+        <f>SIGNs!A130</f>
+        <v>129</v>
+      </c>
+      <c r="K155" t="s">
+        <v>218</v>
+      </c>
+      <c r="L155" t="s">
+        <v>218</v>
+      </c>
+      <c r="M155" t="s">
+        <v>218</v>
+      </c>
+      <c r="N155" t="s">
+        <v>218</v>
+      </c>
+      <c r="O155" t="s">
+        <v>218</v>
+      </c>
+      <c r="P155">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>255</v>
+      </c>
+      <c r="U155">
+        <v>16</v>
+      </c>
+      <c r="V155" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W155" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X155" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="156" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C156">
+        <f>SIGNs!A131</f>
+        <v>130</v>
+      </c>
+      <c r="K156" t="s">
+        <v>218</v>
+      </c>
+      <c r="L156" t="s">
+        <v>218</v>
+      </c>
+      <c r="M156" t="s">
+        <v>218</v>
+      </c>
+      <c r="N156" t="s">
+        <v>218</v>
+      </c>
+      <c r="O156" t="s">
+        <v>218</v>
+      </c>
+      <c r="P156">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>255</v>
+      </c>
+      <c r="U156">
+        <v>16</v>
+      </c>
+      <c r="V156" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W156" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X156" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="157" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C157">
         <f>SIGNs!A149</f>
         <v>148</v>
       </c>
-      <c r="P155">
-        <v>0</v>
-      </c>
-      <c r="Q155" t="s">
+      <c r="K157" t="b">
+        <v>0</v>
+      </c>
+      <c r="L157" t="b">
+        <v>1</v>
+      </c>
+      <c r="M157" t="b">
+        <v>0</v>
+      </c>
+      <c r="N157" t="b">
+        <v>0</v>
+      </c>
+      <c r="O157" t="s">
+        <v>209</v>
+      </c>
+      <c r="P157">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="s">
         <v>214</v>
       </c>
-      <c r="U155">
+      <c r="U157">
         <v>18</v>
       </c>
-    </row>
-    <row r="156" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C156">
+      <c r="V157" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W157" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X157" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="158" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C158">
         <f>SIGNs!A150</f>
         <v>149</v>
       </c>
-      <c r="P156">
-        <v>0</v>
-      </c>
-      <c r="Q156" t="s">
+      <c r="K158" t="b">
+        <v>0</v>
+      </c>
+      <c r="L158" t="b">
+        <v>1</v>
+      </c>
+      <c r="M158" t="b">
+        <v>0</v>
+      </c>
+      <c r="N158" t="b">
+        <v>0</v>
+      </c>
+      <c r="O158" t="s">
+        <v>209</v>
+      </c>
+      <c r="P158">
+        <v>0</v>
+      </c>
+      <c r="Q158" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="157" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C157">
+      <c r="U158">
+        <v>18</v>
+      </c>
+      <c r="V158" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W158" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X158" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="159" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C159">
         <f>SIGNs!A151</f>
         <v>150</v>
       </c>
-      <c r="P157">
-        <v>0</v>
-      </c>
-      <c r="Q157" t="s">
+      <c r="K159" t="b">
+        <v>0</v>
+      </c>
+      <c r="L159" t="b">
+        <v>1</v>
+      </c>
+      <c r="M159" t="b">
+        <v>0</v>
+      </c>
+      <c r="N159" t="b">
+        <v>0</v>
+      </c>
+      <c r="O159" t="s">
+        <v>209</v>
+      </c>
+      <c r="P159">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="158" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C158">
+      <c r="U159">
+        <v>18</v>
+      </c>
+      <c r="V159" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W159" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X159" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="160" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C160">
         <f>SIGNs!A152</f>
         <v>151</v>
       </c>
-      <c r="P158">
-        <v>0</v>
-      </c>
-      <c r="Q158" t="s">
+      <c r="K160" t="b">
+        <v>0</v>
+      </c>
+      <c r="L160" t="b">
+        <v>0</v>
+      </c>
+      <c r="M160" t="b">
+        <v>0</v>
+      </c>
+      <c r="N160" t="b">
+        <v>1</v>
+      </c>
+      <c r="O160" t="s">
+        <v>209</v>
+      </c>
+      <c r="P160">
+        <v>0</v>
+      </c>
+      <c r="Q160" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="159" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C159">
+      <c r="U160">
+        <v>18</v>
+      </c>
+      <c r="V160" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W160" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X160" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="161" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C161">
         <f>SIGNs!A153</f>
         <v>152</v>
       </c>
-      <c r="P159">
-        <v>0</v>
-      </c>
-      <c r="Q159" t="s">
+      <c r="O161" t="s">
+        <v>218</v>
+      </c>
+      <c r="P161">
+        <v>0</v>
+      </c>
+      <c r="Q161" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="160" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C160">
+      <c r="U161">
+        <v>18</v>
+      </c>
+      <c r="V161" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W161" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X161" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="162" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C162">
         <f>SIGNs!A154</f>
         <v>153</v>
       </c>
-      <c r="P160">
-        <v>0</v>
-      </c>
-      <c r="Q160" t="s">
+      <c r="P162">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="s">
         <v>226</v>
       </c>
-      <c r="U160">
+      <c r="U162">
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C161">
+    <row r="163" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C163">
         <f>SIGNs!A155</f>
         <v>154</v>
       </c>
-      <c r="P161">
-        <v>0</v>
-      </c>
-      <c r="Q161" t="s">
+      <c r="P163">
+        <v>0</v>
+      </c>
+      <c r="Q163" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="162" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C162">
+    <row r="164" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C164">
         <f>SIGNs!A156</f>
         <v>155</v>
       </c>
-      <c r="P162">
-        <v>0</v>
-      </c>
-      <c r="Q162" t="s">
+      <c r="P164">
+        <v>0</v>
+      </c>
+      <c r="Q164" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="163" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C163">
+    <row r="165" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C165">
         <f>SIGNs!A157</f>
         <v>156</v>
       </c>
-      <c r="P163">
-        <v>0</v>
-      </c>
-      <c r="Q163" t="s">
+      <c r="P165">
+        <v>0</v>
+      </c>
+      <c r="Q165" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="164" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C164">
+    <row r="166" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C166">
         <f>SIGNs!A158</f>
         <v>157</v>
       </c>
-      <c r="P164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C165">
+      <c r="P166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C167">
         <f>SIGNs!A159</f>
         <v>158</v>
       </c>
-      <c r="P165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C166">
-        <f>SIGNs!A160</f>
-        <v>159</v>
-      </c>
-      <c r="P166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C167">
+      <c r="P167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C168">
         <f>SIGNs!A162</f>
         <v>161</v>
-      </c>
-      <c r="P167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C168">
-        <f>SIGNs!A164</f>
-        <v>163</v>
       </c>
       <c r="P168">
         <v>0</v>
@@ -6613,13 +8089,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I163" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:L163 N1 K1:L1 N10:N163" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K138:L163 N1 K1:L1 N10:N135 K10:L135 N138:N163" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"null,True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1 M10:M163" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1 M10:M135 M138:M163" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1 O10:O163" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1 O10:O163 K136:N137" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:X45 V52:X163" xr:uid="{00000000-0002-0000-0000-000006000000}">

</xml_diff>